<commit_message>
set my study in 12/8/2019
</commit_message>
<xml_diff>
--- a/Amir-Learning.xlsx
+++ b/Amir-Learning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>English</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>create a portfolio</t>
+  </si>
+  <si>
+    <t>unit 1 from telegram and …</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,25 +320,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
@@ -554,7 +564,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1813,20 +1823,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC270"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="29" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="29" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="30" max="16384" width="15.44140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -1913,37 +1922,43 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -1955,53 +1970,53 @@
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2012,781 +2027,799 @@
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" s="14"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A20" s="14"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A21" s="14"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A22" s="14"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A23" s="14"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A24" s="14"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A25" s="14"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A26" s="14"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A27" s="14"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A28" s="14"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A29" s="14"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A30" s="14"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A31" s="14"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A32" s="14"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A33" s="14"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A34" s="14"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A35" s="14"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A36" s="14"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A37" s="14"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A38" s="14"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A39" s="14"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A40" s="14"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A41" s="14"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A42" s="14"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A43" s="14"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A44" s="14"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A45" s="14"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A46" s="14"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A47" s="14"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A48" s="14"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A49" s="14"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A50" s="14"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A51" s="14"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A52" s="14"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A53" s="14"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A54" s="14"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A55" s="14"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A56" s="14"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A57" s="14"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A58" s="14"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A59" s="14"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A60" s="14"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A61" s="14"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A62" s="14"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A63" s="14"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A64" s="14"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A65" s="14"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A66" s="14"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A67" s="14"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A68" s="14"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A69" s="14"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A70" s="14"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A71" s="14"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A72" s="14"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A73" s="14"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A74" s="14"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A75" s="14"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A76" s="14"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A77" s="14"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A78" s="14"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A79" s="14"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A80" s="14"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A81" s="14"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A82" s="14"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A83" s="14"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A84" s="14"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A85" s="14"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A86" s="14"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A87" s="14"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A88" s="14"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A89" s="14"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A90" s="14"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A91" s="14"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A92" s="14"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A93" s="14"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A94" s="14"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A95" s="14"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A96" s="14"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A97" s="14"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A98" s="14"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A99" s="14"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A100" s="14"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A101" s="14"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A102" s="14"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A103" s="14"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A104" s="14"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A105" s="14"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A106" s="14"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A107" s="14"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A108" s="14"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A109" s="14"/>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A110" s="14"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A111" s="14"/>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A112" s="14"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A113" s="14"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A114" s="14"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A115" s="14"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A116" s="14"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A117" s="14"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A118" s="14"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A119" s="14"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A120" s="14"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A121" s="14"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A122" s="14"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A123" s="14"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A124" s="14"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A125" s="14"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A126" s="14"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A127" s="14"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A128" s="14"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A129" s="14"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A130" s="14"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A131" s="14"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A132" s="14"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A133" s="14"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A134" s="14"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A135" s="14"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A136" s="14"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A137" s="14"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A138" s="14"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A139" s="14"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A140" s="14"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A141" s="14"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A142" s="14"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A143" s="14"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A144" s="14"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A145" s="14"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A146" s="14"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A147" s="14"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A148" s="14"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A149" s="14"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A150" s="14"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A151" s="14"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A152" s="14"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A153" s="14"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A154" s="14"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A155" s="14"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A156" s="14"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A157" s="14"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A158" s="14"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A159" s="14"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A160" s="14"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A161" s="14"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A162" s="14"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A163" s="14"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A164" s="14"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A165" s="14"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A166" s="14"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A167" s="14"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A168" s="14"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A169" s="14"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A170" s="14"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A171" s="14"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A172" s="14"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A173" s="14"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A174" s="14"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A175" s="14"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A176" s="14"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A177" s="14"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A178" s="14"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A179" s="14"/>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A180" s="14"/>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A181" s="14"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A182" s="14"/>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A183" s="14"/>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A184" s="14"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A185" s="14"/>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A186" s="14"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A187" s="14"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A188" s="14"/>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A189" s="14"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A190" s="14"/>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A191" s="14"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A192" s="14"/>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A193" s="14"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A194" s="14"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A195" s="14"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A196" s="14"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A197" s="14"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A198" s="14"/>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A199" s="14"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A200" s="14"/>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A201" s="14"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A202" s="14"/>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A203" s="14"/>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A204" s="14"/>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A205" s="14"/>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A206" s="14"/>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A207" s="14"/>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A208" s="14"/>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A209" s="14"/>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A210" s="14"/>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A211" s="14"/>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A212" s="14"/>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A213" s="14"/>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A214" s="14"/>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A215" s="14"/>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A216" s="14"/>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A217" s="14"/>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A218" s="14"/>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A219" s="14"/>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A220" s="14"/>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A221" s="14"/>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A222" s="14"/>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A223" s="14"/>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A224" s="14"/>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A225" s="14"/>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A226" s="14"/>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A227" s="14"/>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A228" s="14"/>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A229" s="14"/>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A230" s="14"/>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A231" s="14"/>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A232" s="14"/>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A233" s="14"/>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A234" s="14"/>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A235" s="14"/>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A236" s="14"/>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A237" s="14"/>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A238" s="14"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A239" s="14"/>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A240" s="14"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A241" s="14"/>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A242" s="14"/>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A243" s="14"/>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A244" s="14"/>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A245" s="14"/>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A246" s="14"/>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A247" s="14"/>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A248" s="14"/>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A249" s="14"/>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A250" s="14"/>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A251" s="14"/>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A252" s="14"/>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A253" s="14"/>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A254" s="14"/>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A255" s="14"/>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A256" s="14"/>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A257" s="14"/>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A258" s="14"/>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A259" s="14"/>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A260" s="14"/>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A261" s="14"/>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A262" s="14"/>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A263" s="14"/>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A264" s="14"/>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A265" s="14"/>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A266" s="14"/>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A267" s="14"/>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A268" s="14"/>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A269" s="14"/>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A270" s="14"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="13"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="13"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+    </row>
+    <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+    </row>
+    <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+    </row>
+    <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+    </row>
+    <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="13"/>
+    </row>
+    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13"/>
+    </row>
+    <row r="39" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="13"/>
+    </row>
+    <row r="40" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13"/>
+    </row>
+    <row r="41" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13"/>
+    </row>
+    <row r="42" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+    </row>
+    <row r="43" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+    </row>
+    <row r="44" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+    </row>
+    <row r="45" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13"/>
+    </row>
+    <row r="46" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="13"/>
+    </row>
+    <row r="47" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+    </row>
+    <row r="48" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+    </row>
+    <row r="49" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+    </row>
+    <row r="50" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="13"/>
+    </row>
+    <row r="51" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="13"/>
+    </row>
+    <row r="52" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="13"/>
+    </row>
+    <row r="53" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="13"/>
+    </row>
+    <row r="54" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="13"/>
+    </row>
+    <row r="55" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="13"/>
+    </row>
+    <row r="56" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13"/>
+    </row>
+    <row r="57" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="13"/>
+    </row>
+    <row r="58" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="13"/>
+    </row>
+    <row r="59" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="13"/>
+    </row>
+    <row r="60" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="13"/>
+    </row>
+    <row r="61" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="13"/>
+    </row>
+    <row r="62" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="13"/>
+    </row>
+    <row r="63" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="13"/>
+    </row>
+    <row r="64" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="13"/>
+    </row>
+    <row r="65" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="13"/>
+    </row>
+    <row r="66" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="13"/>
+    </row>
+    <row r="67" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="13"/>
+    </row>
+    <row r="68" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="13"/>
+    </row>
+    <row r="69" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="13"/>
+    </row>
+    <row r="70" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="13"/>
+    </row>
+    <row r="71" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="13"/>
+    </row>
+    <row r="72" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="13"/>
+    </row>
+    <row r="73" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="13"/>
+    </row>
+    <row r="74" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="13"/>
+    </row>
+    <row r="75" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="13"/>
+    </row>
+    <row r="76" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="13"/>
+    </row>
+    <row r="77" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="13"/>
+    </row>
+    <row r="78" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="13"/>
+    </row>
+    <row r="79" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="13"/>
+    </row>
+    <row r="80" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="13"/>
+    </row>
+    <row r="81" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="13"/>
+    </row>
+    <row r="82" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="13"/>
+    </row>
+    <row r="83" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="13"/>
+    </row>
+    <row r="84" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="13"/>
+    </row>
+    <row r="85" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="13"/>
+    </row>
+    <row r="86" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="13"/>
+    </row>
+    <row r="87" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="13"/>
+    </row>
+    <row r="88" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="13"/>
+    </row>
+    <row r="89" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="13"/>
+    </row>
+    <row r="90" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="13"/>
+    </row>
+    <row r="91" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="13"/>
+    </row>
+    <row r="92" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="13"/>
+    </row>
+    <row r="93" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="13"/>
+    </row>
+    <row r="94" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="13"/>
+    </row>
+    <row r="95" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="13"/>
+    </row>
+    <row r="96" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="13"/>
+    </row>
+    <row r="97" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="13"/>
+    </row>
+    <row r="98" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="13"/>
+    </row>
+    <row r="99" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="13"/>
+    </row>
+    <row r="100" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="13"/>
+    </row>
+    <row r="101" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="13"/>
+    </row>
+    <row r="102" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="13"/>
+    </row>
+    <row r="103" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="13"/>
+    </row>
+    <row r="104" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="13"/>
+    </row>
+    <row r="105" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="13"/>
+    </row>
+    <row r="106" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="13"/>
+    </row>
+    <row r="107" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="13"/>
+    </row>
+    <row r="108" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="13"/>
+    </row>
+    <row r="109" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="13"/>
+    </row>
+    <row r="110" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="13"/>
+    </row>
+    <row r="111" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="13"/>
+    </row>
+    <row r="112" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="13"/>
+    </row>
+    <row r="113" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="13"/>
+    </row>
+    <row r="114" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="13"/>
+    </row>
+    <row r="115" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="13"/>
+    </row>
+    <row r="116" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="13"/>
+    </row>
+    <row r="117" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="13"/>
+    </row>
+    <row r="118" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="13"/>
+    </row>
+    <row r="119" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="13"/>
+    </row>
+    <row r="120" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="13"/>
+    </row>
+    <row r="121" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="13"/>
+    </row>
+    <row r="122" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="13"/>
+    </row>
+    <row r="123" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="13"/>
+    </row>
+    <row r="124" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="13"/>
+    </row>
+    <row r="125" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="13"/>
+    </row>
+    <row r="126" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="13"/>
+    </row>
+    <row r="127" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="13"/>
+    </row>
+    <row r="128" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="13"/>
+    </row>
+    <row r="129" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="13"/>
+    </row>
+    <row r="130" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="13"/>
+    </row>
+    <row r="131" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="13"/>
+    </row>
+    <row r="132" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="13"/>
+    </row>
+    <row r="133" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="13"/>
+    </row>
+    <row r="134" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="13"/>
+    </row>
+    <row r="135" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="13"/>
+    </row>
+    <row r="136" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="13"/>
+    </row>
+    <row r="137" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="13"/>
+    </row>
+    <row r="138" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="13"/>
+    </row>
+    <row r="139" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="13"/>
+    </row>
+    <row r="140" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="13"/>
+    </row>
+    <row r="141" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="13"/>
+    </row>
+    <row r="142" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="13"/>
+    </row>
+    <row r="143" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="13"/>
+    </row>
+    <row r="144" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="13"/>
+    </row>
+    <row r="145" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="13"/>
+    </row>
+    <row r="146" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="13"/>
+    </row>
+    <row r="147" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="13"/>
+    </row>
+    <row r="148" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="13"/>
+    </row>
+    <row r="149" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="13"/>
+    </row>
+    <row r="150" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="13"/>
+    </row>
+    <row r="151" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="13"/>
+    </row>
+    <row r="152" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="13"/>
+    </row>
+    <row r="153" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="13"/>
+    </row>
+    <row r="154" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="13"/>
+    </row>
+    <row r="155" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="13"/>
+    </row>
+    <row r="156" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="13"/>
+    </row>
+    <row r="157" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="13"/>
+    </row>
+    <row r="158" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="13"/>
+    </row>
+    <row r="159" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="13"/>
+    </row>
+    <row r="160" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="13"/>
+    </row>
+    <row r="161" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="13"/>
+    </row>
+    <row r="162" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="13"/>
+    </row>
+    <row r="163" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="13"/>
+    </row>
+    <row r="164" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="13"/>
+    </row>
+    <row r="165" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="13"/>
+    </row>
+    <row r="166" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="13"/>
+    </row>
+    <row r="167" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="13"/>
+    </row>
+    <row r="168" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="13"/>
+    </row>
+    <row r="169" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="13"/>
+    </row>
+    <row r="170" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="13"/>
+    </row>
+    <row r="171" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="13"/>
+    </row>
+    <row r="172" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="13"/>
+    </row>
+    <row r="173" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="13"/>
+    </row>
+    <row r="174" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="13"/>
+    </row>
+    <row r="175" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="13"/>
+    </row>
+    <row r="176" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="13"/>
+    </row>
+    <row r="177" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="13"/>
+    </row>
+    <row r="178" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="13"/>
+    </row>
+    <row r="179" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="13"/>
+    </row>
+    <row r="180" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="13"/>
+    </row>
+    <row r="181" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="13"/>
+    </row>
+    <row r="182" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="13"/>
+    </row>
+    <row r="183" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="13"/>
+    </row>
+    <row r="184" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="13"/>
+    </row>
+    <row r="185" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="13"/>
+    </row>
+    <row r="186" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="13"/>
+    </row>
+    <row r="187" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="13"/>
+    </row>
+    <row r="188" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="13"/>
+    </row>
+    <row r="189" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="13"/>
+    </row>
+    <row r="190" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="13"/>
+    </row>
+    <row r="191" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="13"/>
+    </row>
+    <row r="192" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="13"/>
+    </row>
+    <row r="193" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="13"/>
+    </row>
+    <row r="194" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="13"/>
+    </row>
+    <row r="195" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="13"/>
+    </row>
+    <row r="196" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="13"/>
+    </row>
+    <row r="197" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="13"/>
+    </row>
+    <row r="198" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="13"/>
+    </row>
+    <row r="199" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="13"/>
+    </row>
+    <row r="200" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="13"/>
+    </row>
+    <row r="201" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="13"/>
+    </row>
+    <row r="202" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="13"/>
+    </row>
+    <row r="203" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="13"/>
+    </row>
+    <row r="204" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="13"/>
+    </row>
+    <row r="205" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="13"/>
+    </row>
+    <row r="206" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="13"/>
+    </row>
+    <row r="207" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="13"/>
+    </row>
+    <row r="208" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="13"/>
+    </row>
+    <row r="209" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="13"/>
+    </row>
+    <row r="210" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="13"/>
+    </row>
+    <row r="211" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="13"/>
+    </row>
+    <row r="212" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="13"/>
+    </row>
+    <row r="213" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="13"/>
+    </row>
+    <row r="214" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="13"/>
+    </row>
+    <row r="215" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="13"/>
+    </row>
+    <row r="216" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="13"/>
+    </row>
+    <row r="217" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="13"/>
+    </row>
+    <row r="218" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="13"/>
+    </row>
+    <row r="219" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="13"/>
+    </row>
+    <row r="220" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="13"/>
+    </row>
+    <row r="221" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="13"/>
+    </row>
+    <row r="222" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="13"/>
+    </row>
+    <row r="223" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="13"/>
+    </row>
+    <row r="224" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="13"/>
+    </row>
+    <row r="225" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="13"/>
+    </row>
+    <row r="226" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="13"/>
+    </row>
+    <row r="227" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="13"/>
+    </row>
+    <row r="228" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="13"/>
+    </row>
+    <row r="229" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="13"/>
+    </row>
+    <row r="230" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="13"/>
+    </row>
+    <row r="231" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="13"/>
+    </row>
+    <row r="232" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="13"/>
+    </row>
+    <row r="233" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="13"/>
+    </row>
+    <row r="234" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="13"/>
+    </row>
+    <row r="235" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="13"/>
+    </row>
+    <row r="236" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="13"/>
+    </row>
+    <row r="237" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="13"/>
+    </row>
+    <row r="238" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="13"/>
+    </row>
+    <row r="239" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="13"/>
+    </row>
+    <row r="240" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="13"/>
+    </row>
+    <row r="241" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="13"/>
+    </row>
+    <row r="242" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="13"/>
+    </row>
+    <row r="243" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="13"/>
+    </row>
+    <row r="244" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="13"/>
+    </row>
+    <row r="245" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="13"/>
+    </row>
+    <row r="246" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="13"/>
+    </row>
+    <row r="247" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="13"/>
+    </row>
+    <row r="248" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="13"/>
+    </row>
+    <row r="249" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="13"/>
+    </row>
+    <row r="250" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="13"/>
+    </row>
+    <row r="251" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="13"/>
+    </row>
+    <row r="252" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="13"/>
+    </row>
+    <row r="253" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A253" s="13"/>
+    </row>
+    <row r="254" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A254" s="13"/>
+    </row>
+    <row r="255" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="13"/>
+    </row>
+    <row r="256" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="13"/>
+    </row>
+    <row r="257" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="13"/>
+    </row>
+    <row r="258" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="13"/>
+    </row>
+    <row r="259" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="13"/>
+    </row>
+    <row r="260" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="13"/>
+    </row>
+    <row r="261" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="13"/>
+    </row>
+    <row r="262" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="13"/>
+    </row>
+    <row r="263" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A263" s="13"/>
+    </row>
+    <row r="264" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A264" s="13"/>
+    </row>
+    <row r="265" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A265" s="13"/>
+    </row>
+    <row r="266" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="13"/>
+    </row>
+    <row r="267" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="13"/>
+    </row>
+    <row r="268" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="13"/>
+    </row>
+    <row r="269" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="13"/>
+    </row>
+    <row r="270" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A270" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2800,7 +2833,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AB1048576"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2922,7 +2955,7 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>SUM(Scheduling!B:B,Scheduling!B1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <f>SUM(Scheduling!C:C,Scheduling!C1)</f>
@@ -3041,17 +3074,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -3114,6 +3147,17 @@
       </c>
       <c r="D5" s="3"/>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
change Hour to minute
</commit_message>
<xml_diff>
--- a/Amir-Learning.xlsx
+++ b/Amir-Learning.xlsx
@@ -563,7 +563,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>390</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:AC270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -1935,7 +1935,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="5">
-        <v>2</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
@@ -1943,7 +1943,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="5">
-        <v>3</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="7">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2953,7 +2953,7 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>SUM(Scheduling!B:B,Scheduling!B1)</f>
-        <v>6</v>
+        <v>390</v>
       </c>
       <c r="B2">
         <f>SUM(Scheduling!C:C,Scheduling!C1)</f>

</xml_diff>